<commit_message>
#302 Fixed "Sales Amount with Discount" calculating
</commit_message>
<xml_diff>
--- a/Docs/Source to target mapping.xlsx
+++ b/Docs/Source to target mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zinyk\source\repos\Northwind_BI_Solution\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69233B6-D1B8-4A01-A545-C375917376DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB72C66-F8FC-4407-8ED3-48373B099390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="558" activeTab="4" xr2:uid="{4088A55A-653F-450D-AAB8-4D657457B3B6}"/>
   </bookViews>
@@ -954,18 +954,6 @@
     <t>exists in Integration.Lineage</t>
   </si>
   <si>
-    <t>JOIN OrderID in Order Details</t>
-  </si>
-  <si>
-    <t>JOIN OrderID in Order Details &amp; JOIN ProductKey in Dimension.Product</t>
-  </si>
-  <si>
-    <t>JOIN CustomerKey in Dimension.Customer</t>
-  </si>
-  <si>
-    <t>JOIN EmployeeKey in Dimension.Employee</t>
-  </si>
-  <si>
     <t>ISNULL 0  &amp; OrderID in Order Details</t>
   </si>
   <si>
@@ -976,15 +964,6 @@
   </si>
   <si>
     <t>ISNULL -1 &amp; exists in Dimension.Employee</t>
-  </si>
-  <si>
-    <t>JOIN OrderID in Order Details &amp; UnitPrice * Discount</t>
-  </si>
-  <si>
-    <t>JOIN OrderID in Order Details &amp; UnitPrice * Quantity</t>
-  </si>
-  <si>
-    <t>JOIN OrderID in Order Details &amp; UnitPrice * ( Quantity - Discount )</t>
   </si>
   <si>
     <t>DATETIME</t>
@@ -1080,6 +1059,27 @@
   </si>
   <si>
     <t>CHECKSUM ( [UnitPrice], [Quantity], [Discount] )</t>
+  </si>
+  <si>
+    <t>Lookup OrderID in Order Details &amp; Lookup ProductKey in Dimension.Product</t>
+  </si>
+  <si>
+    <t>Lookup CustomerKey in Dimension.Customer</t>
+  </si>
+  <si>
+    <t>Lookup EmployeeKey in Dimension.Employee</t>
+  </si>
+  <si>
+    <t>Lookup OrderID in Order Details</t>
+  </si>
+  <si>
+    <t>Lookup OrderID in Order Details &amp; UnitPrice * Discount</t>
+  </si>
+  <si>
+    <t>Lookup OrderID in Order Details &amp; UnitPrice * Quantity</t>
+  </si>
+  <si>
+    <t>Lookup OrderID in Order Details &amp; Quantity * UnitPrice * (1 - Discount)</t>
   </si>
 </sst>
 </file>
@@ -1909,7 +1909,7 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>37</v>
@@ -1982,7 +1982,7 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>13</v>
@@ -2057,7 +2057,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>24</v>
@@ -2128,7 +2128,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>25</v>
@@ -2199,7 +2199,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>14</v>
@@ -2270,7 +2270,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>15</v>
@@ -2341,7 +2341,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>16</v>
@@ -2412,7 +2412,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>26</v>
@@ -2616,16 +2616,16 @@
         <v>116</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -3885,7 +3885,7 @@
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P50" s="3" t="s">
         <v>274</v>
@@ -3924,7 +3924,7 @@
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="O51" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P51" s="3" t="s">
         <v>275</v>
@@ -3963,7 +3963,7 @@
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="P52" s="3" t="s">
         <v>276</v>
@@ -5669,7 +5669,7 @@
         <v>153</v>
       </c>
       <c r="AC27" s="22" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
@@ -5710,7 +5710,7 @@
         <v>153</v>
       </c>
       <c r="AC28" s="23" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
@@ -5751,18 +5751,18 @@
         <v>153</v>
       </c>
       <c r="AC29" s="23" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>175</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>176</v>
@@ -5772,7 +5772,7 @@
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="J30" s="20"/>
       <c r="K30" s="20"/>
@@ -5797,7 +5797,7 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>175</v>
@@ -5831,7 +5831,7 @@
       <c r="M31" s="20"/>
       <c r="N31" s="20"/>
       <c r="O31" s="3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="P31" s="21" t="s">
         <v>13</v>
@@ -5862,13 +5862,13 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>175</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>176</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B33" s="20" t="s">
         <v>177</v>
@@ -5939,7 +5939,7 @@
       <c r="M33" s="20"/>
       <c r="N33" s="20"/>
       <c r="O33" s="3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="P33" s="21" t="s">
         <v>37</v>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="R33" s="21"/>
       <c r="S33" s="21" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="T33" s="20" t="s">
         <v>150</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>177</v>
@@ -6008,7 +6008,7 @@
       <c r="M34" s="20"/>
       <c r="N34" s="20"/>
       <c r="O34" s="3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="P34" s="21" t="s">
         <v>174</v>
@@ -6053,7 +6053,7 @@
       <c r="M35" s="20"/>
       <c r="N35" s="20"/>
       <c r="O35" s="3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="P35" s="21" t="s">
         <v>118</v>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="R35" s="21"/>
       <c r="S35" s="21" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="T35" s="20" t="s">
         <v>150</v>
@@ -6098,13 +6098,13 @@
       <c r="M36" s="20"/>
       <c r="N36" s="20"/>
       <c r="O36" s="3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="P36" s="21" t="s">
         <v>145</v>
       </c>
       <c r="Q36" s="21" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="R36" s="21"/>
       <c r="S36" s="21"/>
@@ -6115,11 +6115,11 @@
         <v>145</v>
       </c>
       <c r="V36" s="20" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="W36" s="20"/>
       <c r="X36" s="25" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="Y36" s="22"/>
       <c r="Z36" s="22"/>
@@ -6129,13 +6129,13 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>177</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>176</v>
@@ -6145,7 +6145,7 @@
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="I37" s="21" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="J37" s="20"/>
       <c r="K37" s="20"/>
@@ -6170,13 +6170,13 @@
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>177</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>176</v>
@@ -6209,13 +6209,13 @@
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>177</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D39" s="20" t="s">
         <v>176</v>
@@ -6255,16 +6255,16 @@
         <v>154</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
@@ -6784,7 +6784,7 @@
       <c r="M54" s="20"/>
       <c r="N54" s="20"/>
       <c r="O54" s="3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="P54" s="3" t="s">
         <v>274</v>
@@ -6823,7 +6823,7 @@
       <c r="M55" s="20"/>
       <c r="N55" s="20"/>
       <c r="O55" s="3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="P55" s="3" t="s">
         <v>275</v>
@@ -6862,7 +6862,7 @@
       <c r="M56" s="20"/>
       <c r="N56" s="20"/>
       <c r="O56" s="3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="P56" s="3" t="s">
         <v>276</v>
@@ -8380,16 +8380,16 @@
         <v>219</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -10772,16 +10772,16 @@
         <v>255</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -11523,16 +11523,16 @@
         <v>259</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -12699,8 +12699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE506E6D-FDB6-42A6-8384-1E788212D2E3}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12847,10 +12847,10 @@
         <v>29</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>305</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -12887,10 +12887,10 @@
         <v>29</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>306</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -12927,10 +12927,10 @@
         <v>29</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>307</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -12944,7 +12944,7 @@
         <v>296</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>301</v>
@@ -12953,7 +12953,7 @@
         <v>296</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -12967,7 +12967,7 @@
         <v>146</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="N7" s="5"/>
     </row>
@@ -12982,7 +12982,7 @@
         <v>297</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>301</v>
@@ -12991,7 +12991,7 @@
         <v>297</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -13005,7 +13005,7 @@
         <v>146</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="N8" s="5"/>
     </row>
@@ -13020,7 +13020,7 @@
         <v>298</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>301</v>
@@ -13029,7 +13029,7 @@
         <v>298</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -13043,7 +13043,7 @@
         <v>146</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="N9" s="5"/>
     </row>
@@ -13067,10 +13067,10 @@
         <v>253</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>304</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -13093,10 +13093,10 @@
         <v>29</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>304</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -13119,10 +13119,10 @@
         <v>253</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>312</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -13145,10 +13145,10 @@
         <v>253</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>313</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -13171,10 +13171,10 @@
         <v>253</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>314</v>
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -13270,16 +13270,16 @@
         <v>255</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -13426,7 +13426,7 @@
         <v>292</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>302</v>
@@ -13435,7 +13435,7 @@
         <v>292</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>12</v>
@@ -13456,16 +13456,16 @@
         <v>255</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H24" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>343</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>

</xml_diff>

<commit_message>
Updated Source to target mapping.xlsx
</commit_message>
<xml_diff>
--- a/Docs/Source to target mapping.xlsx
+++ b/Docs/Source to target mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zinyk\source\repos\Northwind_BI_Solution\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZinukovD\source\repos\Northwind_BI_Solution\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783E6AA2-0426-4EF9-BB13-F3A5B11D5450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1886F2E7-3FF5-4AA5-B8B8-AFB8F731415E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="558" activeTab="4" xr2:uid="{4088A55A-653F-450D-AAB8-4D657457B3B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="558" activeTab="3" xr2:uid="{4088A55A-653F-450D-AAB8-4D657457B3B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="345">
   <si>
     <t>Source</t>
   </si>
@@ -1067,6 +1067,60 @@
   </si>
   <si>
     <t>Lookup OrderID in Order Details &amp; [Quantity] * [UnitPrice] * (1 - [Discount])</t>
+  </si>
+  <si>
+    <t>AllAttributes</t>
+  </si>
+  <si>
+    <t>[MasterCustomerAllAttributes] = (
+			SELECT	*
+			FROM	[mdm].[MasterCustomer] AS subquery
+			WHERE	subquery.[Code] = MC.[Code]
+			FOR JSON PATH, WITHOUT_ARRAY_WRAPPER
+		)
+DQSCustomerAllAttributes = (
+			SELECT	*
+			FROM	[dbo].[NW_Customers] AS subquery
+			WHERE	subquery.[CustomerID_Output] = NWP.[CustomerID_Output]
+			FOR JSON PATH, WITHOUT_ARRAY_WRAPPER
+		)
+(DT_NTEXT)"{\"MDS\":[{\"mdm_masterCustomer\":" + (ISNULL(MasterCustomerAllAttributes) ? (DT_NTEXT)"{}" : MasterCustomerAllAttributes) + (DT_NTEXT)"}],\"DQS\":[{\"dbo_NW_Customers\":" + (ISNULL(DQSCustomerAllAttributes) ? (DT_NTEXT)"{}" : DQSCustomerAllAttributes) + (DT_NTEXT)"}]}"</t>
+  </si>
+  <si>
+    <t>[MasterEmployeeAllAttributes] = (
+			SELECT	*
+			FROM	[mdm].[MasterEmployee] AS subquery
+			WHERE	subquery.[Code] = MC.[Code]
+			FOR JSON PATH, WITHOUT_ARRAY_WRAPPER
+		)
+DQSEmployeeAllAttributes = (
+			SELECT	*
+			FROM	[dbo].[NW_Employees] AS subquery
+			WHERE	subquery.[EmployeeID_Output] = NWP.[EmployeeID_Output]
+			FOR JSON PATH, WITHOUT_ARRAY_WRAPPER
+		)
+(DT_NTEXT)"{\"MDS\":[{\"mdm_masterEmployee\":" + (ISNULL(MasterEmployeeAllAttributes) ? (DT_NTEXT)"{}" : MasterEmployeeAllAttributes) + (DT_NTEXT)"}],\"DQS\":[{\"dbo_NW_Employees\":" + (ISNULL(DQSEmployeeAllAttributes) ? (DT_NTEXT)"{}" : DQSEmployeeAllAttributes) + (DT_NTEXT)"}]}"</t>
+  </si>
+  <si>
+    <t>[MasterProductAllAttributes] = (
+			SELECT	*
+			FROM	[mdm].[MasterProduct] AS subquery
+			WHERE	subquery.[Code] = MP.[Code]
+			FOR JSON PATH, WITHOUT_ARRAY_WRAPPER
+		)
+[DQSProductAllAttributes] = (
+			SELECT	*
+			FROM	[dbo].[NW_Products] AS subquery
+			WHERE	subquery.[ProductID_Output] = NWP.[ProductID_Output]
+			FOR JSON PATH, WITHOUT_ARRAY_WRAPPER
+		)
+[DQSCategoryAllAttributes] = (
+			SELECT	*
+			FROM	[dbo].[NW_Categories] AS subquery
+			WHERE	subquery.[CategoryID_Output] = NWP.[CategoryID_Output]
+			FOR JSON PATH, WITHOUT_ARRAY_WRAPPER
+		)
+(DT_NTEXT)"{\"MDS\":[{\"mdm_masterProduct\":" + (ISNULL(MasterProductAllAttributes) ? (DT_NTEXT)"{}" : MasterProductAllAttributes) + (DT_NTEXT)"}],\"DQS\":[{\"dbo_NW_Products\":" + (ISNULL(DQSProductAllAttributes) ? (DT_NTEXT)"{}" : DQSProductAllAttributes) + (DT_NTEXT)"},{\"dbo_NW_Categories\":" + (ISNULL(DQSCategoryAllAttributes) ? (DT_NTEXT)"{}" : DQSCategoryAllAttributes) + (DT_NTEXT)"}]}"</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1312,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -1344,11 +1398,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="20% — акцент1" xfId="3" builtinId="30"/>
+    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Акцент3 2" xfId="2" xr:uid="{72B9F317-F5C0-45A7-AA7C-0F44C45D1FF6}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{A125878E-94C1-497A-B7A1-BCB52D1AE9BA}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1365,9 +1421,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1405,7 +1461,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1511,7 +1567,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1661,11 +1717,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438DCF2F-B5A9-4CE2-9803-6BD6F67BD7E5}">
-  <dimension ref="A1:AC66"/>
+  <dimension ref="A1:AC67"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="R12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,7 +1751,7 @@
     <col min="24" max="24" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="40.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="30" max="16384" width="9.140625" style="4"/>
@@ -2476,17 +2532,17 @@
       <c r="Y12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="Z12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB12" s="10" t="s">
+      <c r="Z12" t="s">
+        <v>341</v>
+      </c>
+      <c r="AA12" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB12" t="s">
         <v>12</v>
       </c>
-      <c r="AC12" s="10" t="s">
-        <v>17</v>
+      <c r="AC12" s="42" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
@@ -2518,12 +2574,14 @@
         <v>10</v>
       </c>
       <c r="Z13" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AA13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AB13" s="10"/>
+      <c r="AB13" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AC13" s="10" t="s">
         <v>17</v>
       </c>
@@ -2557,14 +2615,12 @@
         <v>10</v>
       </c>
       <c r="Z14" s="10" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="AA14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB14" s="10" t="s">
-        <v>12</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="AB14" s="10"/>
       <c r="AC14" s="10" t="s">
         <v>17</v>
       </c>
@@ -2598,36 +2654,28 @@
         <v>10</v>
       </c>
       <c r="Z15" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA15" s="10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="AB15" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC15" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="AC15" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>326</v>
-      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -2643,10 +2691,18 @@
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="10"/>
+      <c r="Y16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB16" s="10" t="s">
+        <v>114</v>
+      </c>
       <c r="AC16" s="10"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
@@ -2654,20 +2710,24 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>102</v>
-      </c>
+      <c r="E17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="3"/>
@@ -2700,10 +2760,10 @@
         <v>59</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -2737,7 +2797,7 @@
         <v>59</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>61</v>
@@ -2774,7 +2834,7 @@
         <v>59</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>61</v>
@@ -2811,10 +2871,10 @@
         <v>59</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
@@ -2848,10 +2908,10 @@
         <v>59</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
@@ -2885,7 +2945,7 @@
         <v>59</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>61</v>
@@ -2922,7 +2982,7 @@
         <v>59</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>61</v>
@@ -2959,10 +3019,10 @@
         <v>59</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
@@ -2996,10 +3056,10 @@
         <v>59</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
@@ -3033,7 +3093,7 @@
         <v>59</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>61</v>
@@ -3070,7 +3130,7 @@
         <v>59</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>61</v>
@@ -3107,10 +3167,10 @@
         <v>59</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -3144,10 +3204,10 @@
         <v>59</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
@@ -3181,7 +3241,7 @@
         <v>59</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>61</v>
@@ -3218,7 +3278,7 @@
         <v>59</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>61</v>
@@ -3255,10 +3315,10 @@
         <v>59</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
@@ -3292,10 +3352,10 @@
         <v>59</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
@@ -3329,7 +3389,7 @@
         <v>59</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L35" s="8" t="s">
         <v>61</v>
@@ -3366,7 +3426,7 @@
         <v>59</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L36" s="8" t="s">
         <v>61</v>
@@ -3403,10 +3463,10 @@
         <v>59</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
@@ -3440,10 +3500,10 @@
         <v>59</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
@@ -3477,7 +3537,7 @@
         <v>59</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>61</v>
@@ -3514,7 +3574,7 @@
         <v>59</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>61</v>
@@ -3551,10 +3611,10 @@
         <v>59</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
@@ -3588,10 +3648,10 @@
         <v>59</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
@@ -3625,7 +3685,7 @@
         <v>59</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>61</v>
@@ -3662,7 +3722,7 @@
         <v>59</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>61</v>
@@ -3699,10 +3759,10 @@
         <v>59</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -3736,10 +3796,10 @@
         <v>59</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -3773,7 +3833,7 @@
         <v>59</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L47" s="8" t="s">
         <v>61</v>
@@ -3810,7 +3870,7 @@
         <v>59</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L48" s="8" t="s">
         <v>61</v>
@@ -3847,7 +3907,7 @@
         <v>59</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L49" s="8" t="s">
         <v>61</v>
@@ -3880,24 +3940,22 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
+      <c r="J50" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L50" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
-      <c r="O50" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="P50" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q50" s="3" t="s">
-        <v>273</v>
-      </c>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
-      <c r="S50" s="3" t="s">
-        <v>275</v>
-      </c>
+      <c r="S50" s="3"/>
       <c r="T50" s="5"/>
       <c r="U50" s="5"/>
       <c r="V50" s="5"/>
@@ -3928,7 +3986,7 @@
         <v>306</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q51" s="3" t="s">
         <v>273</v>
@@ -3967,14 +4025,14 @@
         <v>306</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R52" s="3"/>
       <c r="S52" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T52" s="5"/>
       <c r="U52" s="5"/>
@@ -3997,25 +4055,27 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
+      <c r="O53" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q53" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="R53" s="3"/>
-      <c r="S53" s="3"/>
-      <c r="T53" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="U53" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="V53" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="S53" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
       <c r="W53" s="5"/>
       <c r="X53" s="5"/>
       <c r="Y53" s="10"/>
@@ -4048,10 +4108,10 @@
         <v>38</v>
       </c>
       <c r="U54" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V54" s="8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="W54" s="5"/>
       <c r="X54" s="5"/>
@@ -4085,10 +4145,10 @@
         <v>38</v>
       </c>
       <c r="U55" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V55" s="8" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="W55" s="5"/>
       <c r="X55" s="5"/>
@@ -4122,10 +4182,10 @@
         <v>38</v>
       </c>
       <c r="U56" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V56" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="W56" s="5"/>
       <c r="X56" s="5"/>
@@ -4159,7 +4219,7 @@
         <v>38</v>
       </c>
       <c r="U57" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V57" s="8" t="s">
         <v>29</v>
@@ -4196,10 +4256,10 @@
         <v>38</v>
       </c>
       <c r="U58" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V58" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W58" s="5"/>
       <c r="X58" s="5"/>
@@ -4233,10 +4293,10 @@
         <v>38</v>
       </c>
       <c r="U59" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V59" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="W59" s="5"/>
       <c r="X59" s="5"/>
@@ -4270,10 +4330,10 @@
         <v>38</v>
       </c>
       <c r="U60" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V60" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="W60" s="5"/>
       <c r="X60" s="5"/>
@@ -4307,10 +4367,10 @@
         <v>38</v>
       </c>
       <c r="U61" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V61" s="8" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="W61" s="5"/>
       <c r="X61" s="5"/>
@@ -4344,10 +4404,10 @@
         <v>38</v>
       </c>
       <c r="U62" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V62" s="8" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="W62" s="5"/>
       <c r="X62" s="5"/>
@@ -4377,18 +4437,16 @@
       <c r="Q63" s="3"/>
       <c r="R63" s="3"/>
       <c r="S63" s="3"/>
-      <c r="T63" s="5" t="s">
+      <c r="T63" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U63" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="V63" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="W63" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="U63" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="V63" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W63" s="5"/>
       <c r="X63" s="5"/>
       <c r="Y63" s="10"/>
       <c r="Z63" s="10"/>
@@ -4416,16 +4474,18 @@
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
       <c r="S64" s="3"/>
-      <c r="T64" s="8" t="s">
+      <c r="T64" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="U64" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="V64" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="W64" s="5"/>
+      <c r="U64" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="V64" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W64" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="X64" s="5"/>
       <c r="Y64" s="10"/>
       <c r="Z64" s="10"/>
@@ -4457,10 +4517,10 @@
         <v>38</v>
       </c>
       <c r="U65" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V65" s="8" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="W65" s="5"/>
       <c r="X65" s="5"/>
@@ -4490,24 +4550,61 @@
       <c r="Q66" s="3"/>
       <c r="R66" s="3"/>
       <c r="S66" s="3"/>
-      <c r="T66" s="5" t="s">
+      <c r="T66" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U66" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V66" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="W66" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="U66" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="V66" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W66" s="5"/>
       <c r="X66" s="5"/>
       <c r="Y66" s="10"/>
       <c r="Z66" s="10"/>
       <c r="AA66" s="10"/>
       <c r="AB66" s="10"/>
       <c r="AC66" s="10"/>
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="U67" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V67" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W67" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="X67" s="5"/>
+      <c r="Y67" s="10"/>
+      <c r="Z67" s="10"/>
+      <c r="AA67" s="10"/>
+      <c r="AB67" s="10"/>
+      <c r="AC67" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AC2" xr:uid="{1F5E2F5F-C2D6-459F-93D3-DF31ABBA7353}"/>
@@ -7464,11 +7561,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A737B06D-3CA5-4C46-8E57-2C9FAE17A6AF}">
-  <dimension ref="A1:AC62"/>
+  <dimension ref="A1:AC63"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="AB10" sqref="AA10:AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7499,9 +7596,9 @@
     <col min="24" max="24" width="44" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="40.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="58.140625" style="4" customWidth="1"/>
     <col min="30" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -8104,8 +8201,8 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
@@ -8114,17 +8211,17 @@
       <c r="Y10" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="Z10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB10" s="10" t="s">
+      <c r="Z10" t="s">
+        <v>341</v>
+      </c>
+      <c r="AA10" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB10" t="s">
         <v>12</v>
       </c>
-      <c r="AC10" s="10" t="s">
-        <v>17</v>
+      <c r="AC10" s="42" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -8156,12 +8253,14 @@
         <v>185</v>
       </c>
       <c r="Z11" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AA11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AB11" s="10"/>
+      <c r="AB11" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AC11" s="10" t="s">
         <v>17</v>
       </c>
@@ -8195,14 +8294,12 @@
         <v>185</v>
       </c>
       <c r="Z12" s="10" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="AA12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB12" s="10" t="s">
-        <v>12</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="AB12" s="10"/>
       <c r="AC12" s="10" t="s">
         <v>17</v>
       </c>
@@ -8236,81 +8333,55 @@
         <v>185</v>
       </c>
       <c r="Z13" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA13" s="10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="AB13" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC13" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="AC13" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>61</v>
-      </c>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="N14" s="5"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
-      <c r="T14" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="V14" s="5" t="s">
-        <v>192</v>
-      </c>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14" s="10"/>
+      <c r="Y14" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB14" s="10" t="s">
+        <v>114</v>
+      </c>
       <c r="AC14" s="10"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
@@ -8321,16 +8392,16 @@
         <v>219</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>219</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>192</v>
@@ -8343,20 +8414,20 @@
         <v>193</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>61</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>269</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>192</v>
@@ -8367,7 +8438,7 @@
         <v>191</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="V15" s="5" t="s">
         <v>192</v>
@@ -8381,38 +8452,64 @@
       <c r="AC15" s="10"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="E16" s="3" t="s">
         <v>219</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>324</v>
+        <v>189</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
+      <c r="N16" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
       <c r="Y16" s="10"/>
@@ -8426,27 +8523,31 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="L17" s="8" t="s">
+      <c r="E17" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="H17" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
       <c r="V17" s="5"/>
@@ -8472,10 +8573,10 @@
         <v>193</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -8509,7 +8610,7 @@
         <v>193</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>61</v>
@@ -8546,7 +8647,7 @@
         <v>193</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>61</v>
@@ -8583,10 +8684,10 @@
         <v>193</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>192</v>
+        <v>61</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
@@ -8620,10 +8721,10 @@
         <v>193</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>61</v>
+        <v>192</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
@@ -8657,7 +8758,7 @@
         <v>193</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>61</v>
@@ -8694,7 +8795,7 @@
         <v>193</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>61</v>
@@ -8731,10 +8832,10 @@
         <v>193</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>192</v>
+        <v>61</v>
       </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
@@ -8768,10 +8869,10 @@
         <v>193</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>61</v>
+        <v>192</v>
       </c>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
@@ -8805,7 +8906,7 @@
         <v>193</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>61</v>
@@ -8842,7 +8943,7 @@
         <v>193</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>61</v>
@@ -8879,10 +8980,10 @@
         <v>193</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -8916,10 +9017,10 @@
         <v>193</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
@@ -8953,7 +9054,7 @@
         <v>193</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>61</v>
@@ -8990,7 +9091,7 @@
         <v>193</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>61</v>
@@ -9027,10 +9128,10 @@
         <v>193</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>149</v>
+        <v>61</v>
       </c>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
@@ -9064,10 +9165,10 @@
         <v>193</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>61</v>
+        <v>149</v>
       </c>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
@@ -9101,7 +9202,7 @@
         <v>193</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L35" s="8" t="s">
         <v>61</v>
@@ -9138,7 +9239,7 @@
         <v>193</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L36" s="8" t="s">
         <v>61</v>
@@ -9175,10 +9276,10 @@
         <v>193</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>85</v>
+        <v>218</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
@@ -9212,10 +9313,10 @@
         <v>193</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
@@ -9249,7 +9350,7 @@
         <v>193</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>61</v>
@@ -9286,7 +9387,7 @@
         <v>193</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>61</v>
@@ -9323,10 +9424,10 @@
         <v>193</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
@@ -9360,10 +9461,10 @@
         <v>193</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
@@ -9397,7 +9498,7 @@
         <v>193</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>61</v>
@@ -9434,7 +9535,7 @@
         <v>193</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>61</v>
@@ -9471,7 +9572,7 @@
         <v>193</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="L45" s="8" t="s">
         <v>61</v>
@@ -9504,24 +9605,22 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
+      <c r="J46" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
-      <c r="O46" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="P46" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q46" s="3" t="s">
-        <v>273</v>
-      </c>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
       <c r="R46" s="10"/>
-      <c r="S46" s="14" t="s">
-        <v>275</v>
-      </c>
+      <c r="S46" s="10"/>
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
       <c r="V46" s="5"/>
@@ -9552,7 +9651,7 @@
         <v>269</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q47" s="3" t="s">
         <v>273</v>
@@ -9591,14 +9690,14 @@
         <v>269</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R48" s="10"/>
-      <c r="S48" s="10" t="s">
-        <v>276</v>
+      <c r="S48" s="14" t="s">
+        <v>275</v>
       </c>
       <c r="T48" s="5"/>
       <c r="U48" s="5"/>
@@ -9621,25 +9720,27 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
       <c r="M49" s="5"/>
       <c r="N49" s="5"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
+      <c r="O49" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="R49" s="10"/>
-      <c r="S49" s="10"/>
-      <c r="T49" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="U49" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="V49" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="S49" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
       <c r="W49" s="5"/>
       <c r="X49" s="5"/>
       <c r="Y49" s="10"/>
@@ -9672,10 +9773,10 @@
         <v>191</v>
       </c>
       <c r="U50" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V50" s="8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="W50" s="5"/>
       <c r="X50" s="5"/>
@@ -9709,10 +9810,10 @@
         <v>191</v>
       </c>
       <c r="U51" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V51" s="8" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="W51" s="5"/>
       <c r="X51" s="5"/>
@@ -9746,10 +9847,10 @@
         <v>191</v>
       </c>
       <c r="U52" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V52" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="W52" s="5"/>
       <c r="X52" s="5"/>
@@ -9783,7 +9884,7 @@
         <v>191</v>
       </c>
       <c r="U53" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V53" s="8" t="s">
         <v>29</v>
@@ -9820,10 +9921,10 @@
         <v>191</v>
       </c>
       <c r="U54" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V54" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W54" s="5"/>
       <c r="X54" s="5"/>
@@ -9857,10 +9958,10 @@
         <v>191</v>
       </c>
       <c r="U55" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V55" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="W55" s="5"/>
       <c r="X55" s="5"/>
@@ -9894,10 +9995,10 @@
         <v>191</v>
       </c>
       <c r="U56" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V56" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="W56" s="5"/>
       <c r="X56" s="5"/>
@@ -9931,10 +10032,10 @@
         <v>191</v>
       </c>
       <c r="U57" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V57" s="8" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="W57" s="5"/>
       <c r="X57" s="5"/>
@@ -9968,10 +10069,10 @@
         <v>191</v>
       </c>
       <c r="U58" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V58" s="8" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="W58" s="5"/>
       <c r="X58" s="5"/>
@@ -10001,18 +10102,16 @@
       <c r="Q59" s="3"/>
       <c r="R59" s="10"/>
       <c r="S59" s="10"/>
-      <c r="T59" s="5" t="s">
+      <c r="T59" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="U59" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="V59" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="W59" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="U59" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="V59" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W59" s="5"/>
       <c r="X59" s="5"/>
       <c r="Y59" s="10"/>
       <c r="Z59" s="10"/>
@@ -10040,16 +10139,18 @@
       <c r="Q60" s="3"/>
       <c r="R60" s="10"/>
       <c r="S60" s="10"/>
-      <c r="T60" s="8" t="s">
+      <c r="T60" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="U60" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="V60" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="W60" s="5"/>
+      <c r="U60" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="V60" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W60" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="X60" s="5"/>
       <c r="Y60" s="10"/>
       <c r="Z60" s="10"/>
@@ -10081,10 +10182,10 @@
         <v>191</v>
       </c>
       <c r="U61" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V61" s="8" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="W61" s="5"/>
       <c r="X61" s="5"/>
@@ -10114,24 +10215,61 @@
       <c r="Q62" s="3"/>
       <c r="R62" s="10"/>
       <c r="S62" s="10"/>
-      <c r="T62" s="5" t="s">
+      <c r="T62" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="U62" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V62" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="W62" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="U62" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="V62" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W62" s="5"/>
       <c r="X62" s="5"/>
       <c r="Y62" s="10"/>
       <c r="Z62" s="10"/>
       <c r="AA62" s="10"/>
       <c r="AB62" s="10"/>
       <c r="AC62" s="10"/>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="10"/>
+      <c r="S63" s="10"/>
+      <c r="T63" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="U63" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V63" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W63" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="X63" s="5"/>
+      <c r="Y63" s="10"/>
+      <c r="Z63" s="10"/>
+      <c r="AA63" s="10"/>
+      <c r="AB63" s="10"/>
+      <c r="AC63" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AC2" xr:uid="{02CC11CA-5403-4028-895D-6209F46F2C79}"/>
@@ -10150,11 +10288,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A4499F-EBCA-4E9B-AE48-94E9136B2D31}">
-  <dimension ref="A1:AC58"/>
+  <dimension ref="A1:AC59"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
+      <selection pane="bottomLeft" activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10185,9 +10323,9 @@
     <col min="24" max="24" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="40.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="63.140625" style="4" customWidth="1"/>
     <col min="30" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -10603,11 +10741,11 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -10617,48 +10755,36 @@
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
+      <c r="X7" s="29"/>
       <c r="Y7" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="Z7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB7" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC7" s="10"/>
+      <c r="Z7" t="s">
+        <v>341</v>
+      </c>
+      <c r="AA7" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC7" s="42" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>257</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>257</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>29</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="3"/>
@@ -10671,10 +10797,18 @@
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="10"/>
-      <c r="AB8" s="10"/>
+      <c r="Y8" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB8" s="10" t="s">
+        <v>114</v>
+      </c>
       <c r="AC8" s="10"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
@@ -10685,19 +10819,19 @@
         <v>251</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>250</v>
+        <v>29</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>251</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>250</v>
+        <v>29</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -10723,35 +10857,39 @@
       <c r="AC9" s="10"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3" t="s">
+      <c r="A10" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="C10" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
@@ -10768,11 +10906,21 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>329</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -10781,8 +10929,8 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
@@ -10804,15 +10952,9 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="3"/>
@@ -10845,10 +10987,10 @@
         <v>228</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -10882,7 +11024,7 @@
         <v>228</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>61</v>
@@ -10919,7 +11061,7 @@
         <v>228</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>61</v>
@@ -10956,10 +11098,10 @@
         <v>228</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
@@ -10993,10 +11135,10 @@
         <v>228</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
@@ -11030,7 +11172,7 @@
         <v>228</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>61</v>
@@ -11067,7 +11209,7 @@
         <v>228</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>61</v>
@@ -11104,10 +11246,10 @@
         <v>228</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
@@ -11141,10 +11283,10 @@
         <v>228</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
@@ -11178,7 +11320,7 @@
         <v>228</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>61</v>
@@ -11215,7 +11357,7 @@
         <v>228</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>61</v>
@@ -11252,7 +11394,7 @@
         <v>228</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>101</v>
+        <v>244</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>61</v>
@@ -11285,24 +11427,22 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
+      <c r="J25" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>273</v>
-      </c>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
       <c r="R25" s="10"/>
-      <c r="S25" s="14" t="s">
-        <v>275</v>
-      </c>
+      <c r="S25" s="10"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
@@ -11333,7 +11473,7 @@
         <v>268</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>273</v>
@@ -11372,14 +11512,14 @@
         <v>268</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R27" s="10"/>
-      <c r="S27" s="10" t="s">
-        <v>276</v>
+      <c r="S27" s="14" t="s">
+        <v>275</v>
       </c>
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
@@ -11402,27 +11542,29 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
+      <c r="O28" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>274</v>
+      </c>
       <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="U28" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="V28" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
+      <c r="S28" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
       <c r="Y28" s="10"/>
       <c r="Z28" s="10"/>
       <c r="AA28" s="10"/>
@@ -11453,10 +11595,10 @@
         <v>227</v>
       </c>
       <c r="U29" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V29" s="8" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="W29" s="8"/>
       <c r="X29" s="8"/>
@@ -11490,10 +11632,10 @@
         <v>227</v>
       </c>
       <c r="U30" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V30" s="8" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="W30" s="8"/>
       <c r="X30" s="8"/>
@@ -11527,10 +11669,10 @@
         <v>227</v>
       </c>
       <c r="U31" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V31" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="W31" s="8"/>
       <c r="X31" s="8"/>
@@ -11564,7 +11706,7 @@
         <v>227</v>
       </c>
       <c r="U32" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V32" s="8" t="s">
         <v>29</v>
@@ -11601,10 +11743,10 @@
         <v>227</v>
       </c>
       <c r="U33" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V33" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W33" s="8"/>
       <c r="X33" s="8"/>
@@ -11638,10 +11780,10 @@
         <v>227</v>
       </c>
       <c r="U34" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V34" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
@@ -11675,7 +11817,7 @@
         <v>227</v>
       </c>
       <c r="U35" s="8" t="s">
-        <v>226</v>
+        <v>46</v>
       </c>
       <c r="V35" s="8" t="s">
         <v>29</v>
@@ -11712,10 +11854,10 @@
         <v>227</v>
       </c>
       <c r="U36" s="8" t="s">
-        <v>47</v>
+        <v>226</v>
       </c>
       <c r="V36" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="W36" s="8"/>
       <c r="X36" s="8"/>
@@ -11749,10 +11891,10 @@
         <v>227</v>
       </c>
       <c r="U37" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V37" s="8" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="W37" s="8"/>
       <c r="X37" s="8"/>
@@ -11786,10 +11928,10 @@
         <v>227</v>
       </c>
       <c r="U38" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V38" s="8" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="W38" s="8"/>
       <c r="X38" s="8"/>
@@ -11819,19 +11961,17 @@
       <c r="Q39" s="3"/>
       <c r="R39" s="10"/>
       <c r="S39" s="10"/>
-      <c r="T39" s="5" t="s">
+      <c r="T39" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="U39" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="V39" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="W39" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="X39" s="5"/>
+      <c r="U39" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="V39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
       <c r="Y39" s="10"/>
       <c r="Z39" s="10"/>
       <c r="AA39" s="10"/>
@@ -11858,17 +11998,19 @@
       <c r="Q40" s="3"/>
       <c r="R40" s="10"/>
       <c r="S40" s="10"/>
-      <c r="T40" s="8" t="s">
+      <c r="T40" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="U40" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="V40" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
+      <c r="U40" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="V40" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W40" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="X40" s="5"/>
       <c r="Y40" s="10"/>
       <c r="Z40" s="10"/>
       <c r="AA40" s="10"/>
@@ -11899,10 +12041,10 @@
         <v>227</v>
       </c>
       <c r="U41" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V41" s="8" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="W41" s="8"/>
       <c r="X41" s="8"/>
@@ -11932,19 +12074,17 @@
       <c r="Q42" s="3"/>
       <c r="R42" s="10"/>
       <c r="S42" s="10"/>
-      <c r="T42" s="5" t="s">
+      <c r="T42" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="U42" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V42" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="W42" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="X42" s="5"/>
+      <c r="U42" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="V42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
       <c r="Y42" s="10"/>
       <c r="Z42" s="10"/>
       <c r="AA42" s="10"/>
@@ -11952,59 +12092,37 @@
       <c r="AC42" s="10"/>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
       <c r="I43" s="3"/>
-      <c r="J43" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
       <c r="M43" s="5"/>
-      <c r="N43" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="O43" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="P43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q43" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="N43" s="5"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5"/>
-      <c r="V43" s="5"/>
-      <c r="W43" s="5"/>
+      <c r="T43" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="U43" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V43" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W43" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="X43" s="5"/>
       <c r="Y43" s="10"/>
       <c r="Z43" s="10"/>
@@ -12020,19 +12138,19 @@
         <v>255</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>255</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>12</v>
@@ -12042,20 +12160,20 @@
         <v>229</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="O44" s="3" t="s">
         <v>266</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>39</v>
@@ -12081,30 +12199,46 @@
         <v>255</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>259</v>
+        <v>104</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>255</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="H45" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="I45" s="3"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
+      <c r="J45" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
+      <c r="N45" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="R45" s="10"/>
       <c r="S45" s="10"/>
       <c r="T45" s="5"/>
@@ -12119,25 +12253,29 @@
       <c r="AC45" s="10"/>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="A46" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>259</v>
+      </c>
       <c r="E46" s="3" t="s">
         <v>255</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>324</v>
+        <v>260</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>330</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
@@ -12146,8 +12284,8 @@
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="10"/>
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
       <c r="V46" s="5"/>
@@ -12164,27 +12302,31 @@
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="K47" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="L47" s="8" t="s">
+      <c r="E47" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="H47" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
       <c r="Q47" s="3"/>
-      <c r="R47" s="10"/>
-      <c r="S47" s="10"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
       <c r="T47" s="5"/>
       <c r="U47" s="5"/>
       <c r="V47" s="5"/>
@@ -12210,10 +12352,10 @@
         <v>229</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
@@ -12247,7 +12389,7 @@
         <v>229</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L49" s="8" t="s">
         <v>61</v>
@@ -12284,7 +12426,7 @@
         <v>229</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L50" s="8" t="s">
         <v>61</v>
@@ -12321,10 +12463,10 @@
         <v>229</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
@@ -12358,10 +12500,10 @@
         <v>229</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
@@ -12395,7 +12537,7 @@
         <v>229</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L53" s="8" t="s">
         <v>61</v>
@@ -12432,7 +12574,7 @@
         <v>229</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L54" s="8" t="s">
         <v>61</v>
@@ -12469,7 +12611,7 @@
         <v>229</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>101</v>
+        <v>249</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>61</v>
@@ -12502,24 +12644,22 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
+      <c r="J56" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L56" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
-      <c r="O56" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="P56" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q56" s="3" t="s">
-        <v>273</v>
-      </c>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
       <c r="R56" s="10"/>
-      <c r="S56" s="14" t="s">
-        <v>275</v>
-      </c>
+      <c r="S56" s="10"/>
       <c r="T56" s="5"/>
       <c r="U56" s="5"/>
       <c r="V56" s="5"/>
@@ -12550,7 +12690,7 @@
         <v>266</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q57" s="3" t="s">
         <v>273</v>
@@ -12589,14 +12729,14 @@
         <v>266</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R58" s="10"/>
-      <c r="S58" s="10" t="s">
-        <v>276</v>
+      <c r="S58" s="14" t="s">
+        <v>275</v>
       </c>
       <c r="T58" s="5"/>
       <c r="U58" s="5"/>
@@ -12608,6 +12748,45 @@
       <c r="AA58" s="10"/>
       <c r="AB58" s="10"/>
       <c r="AC58" s="10"/>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q59" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="R59" s="10"/>
+      <c r="S59" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5"/>
+      <c r="V59" s="5"/>
+      <c r="W59" s="5"/>
+      <c r="X59" s="5"/>
+      <c r="Y59" s="10"/>
+      <c r="Z59" s="10"/>
+      <c r="AA59" s="10"/>
+      <c r="AB59" s="10"/>
+      <c r="AC59" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AC2" xr:uid="{FB1DEB6E-3C3E-4F8F-BD13-8004FC7B4D37}"/>
@@ -12628,7 +12807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE506E6D-FDB6-42A6-8384-1E788212D2E3}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>

</xml_diff>